<commit_message>
Version 13 - ADC values Right aligned. - To avoid overrun errors, ADC buffered values no more readed in ebike_app but in pwm-up interrupt (end of conversion) - Fixed minor bug in main loop timings - PWM freq decreased to 18KHz (all values parametrized in main.h) - Power glitch bug fix (race condition between PWM interrupt and Hall GPIO interrupt) - FOC angle asin_table optimization (thanks to beemac) - PWM Dead Time increased from 1us to 1.5us (OEM firmware uses a value of 3us!)
</commit_message>
<xml_diff>
--- a/CSV-PWM-Table.xlsx
+++ b/CSV-PWM-Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-Smart-EBike\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-Smart-EBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48BE021-B143-4576-8934-1421ACC5FB17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF822B2C-A627-4287-B98B-27BF02E2BA50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="276" windowWidth="22800" windowHeight="12684" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
+    <workbookView xWindow="972" yWindow="324" windowWidth="18972" windowHeight="11136" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
   </bookViews>
   <sheets>
     <sheet name="Midpoint Clamp (CSV PWM)" sheetId="2" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Counter Max</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>Scale</t>
   </si>
   <si>
@@ -68,13 +65,17 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>PWM Freq.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;Hz&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -100,15 +101,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -131,20 +138,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6041,10 +6093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F520312-DA36-4F57-882C-348F0CE3BEC0}">
-  <dimension ref="A1:I259"/>
+  <dimension ref="A1:M259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6052,26 +6104,27 @@
     <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1">
         <f>1/4</f>
         <v>0.25</v>
@@ -6085,18 +6138,26 @@
         <v>0.86629626434835505</v>
       </c>
       <c r="G2">
-        <f>ROUND(H2*256/254,0)</f>
-        <v>212</v>
-      </c>
-      <c r="H2" s="2">
-        <v>210</v>
-      </c>
-      <c r="I2">
-        <f>G2*254/256</f>
-        <v>210.34375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H2/2-7</f>
+        <v>215</v>
+      </c>
+      <c r="H2" s="6">
+        <v>444</v>
+      </c>
+      <c r="I2" s="4">
+        <f>16000000/(H2*2)</f>
+        <v>18018.018018018018</v>
+      </c>
+      <c r="L2">
+        <f>TRUNC(254*G2/256)</f>
+        <v>213</v>
+      </c>
+      <c r="M2">
+        <f>H2/2-L2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -6107,7 +6168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>65</v>
       </c>
@@ -6133,10 +6194,10 @@
       </c>
       <c r="G4">
         <f>ROUND(D4*$G$2,0)</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>66</v>
       </c>
@@ -6162,10 +6223,10 @@
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G68" si="5">ROUND(D5*$G$2,0)</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>67</v>
       </c>
@@ -6191,10 +6252,10 @@
       </c>
       <c r="G6">
         <f t="shared" si="5"/>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>68</v>
       </c>
@@ -6220,10 +6281,10 @@
       </c>
       <c r="G7">
         <f t="shared" si="5"/>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>69</v>
       </c>
@@ -6249,10 +6310,10 @@
       </c>
       <c r="G8">
         <f t="shared" si="5"/>
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>70</v>
       </c>
@@ -6278,10 +6339,10 @@
       </c>
       <c r="G9">
         <f t="shared" si="5"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>71</v>
       </c>
@@ -6307,10 +6368,10 @@
       </c>
       <c r="G10">
         <f t="shared" si="5"/>
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>72</v>
       </c>
@@ -6336,10 +6397,10 @@
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>73</v>
       </c>
@@ -6365,10 +6426,10 @@
       </c>
       <c r="G12">
         <f t="shared" si="5"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>74</v>
       </c>
@@ -6394,10 +6455,10 @@
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>75</v>
       </c>
@@ -6423,10 +6484,10 @@
       </c>
       <c r="G14">
         <f t="shared" si="5"/>
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>76</v>
       </c>
@@ -6452,10 +6513,10 @@
       </c>
       <c r="G15">
         <f t="shared" si="5"/>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>77</v>
       </c>
@@ -6481,7 +6542,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -6510,7 +6571,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -6538,8 +6599,8 @@
         <v>254</v>
       </c>
       <c r="G18">
-        <f>ROUND(D18*$G$2,0)</f>
-        <v>211</v>
+        <f t="shared" si="5"/>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -6568,7 +6629,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -6597,7 +6658,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -6626,7 +6687,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -6655,7 +6716,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -6684,7 +6745,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -6713,7 +6774,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -6742,7 +6803,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -6771,7 +6832,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -6800,7 +6861,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -6828,8 +6889,8 @@
         <v>254</v>
       </c>
       <c r="G28">
-        <f>ROUND(D28*$G$2,0)</f>
-        <v>211</v>
+        <f t="shared" si="5"/>
+        <v>214</v>
       </c>
       <c r="I28" t="s">
         <v>6</v>
@@ -6861,7 +6922,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I29" t="s">
         <v>5</v>
@@ -6893,7 +6954,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I30" t="s">
         <v>4</v>
@@ -6925,7 +6986,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I31" t="s">
         <v>1</v>
@@ -6957,7 +7018,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -6986,7 +7047,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -7015,7 +7076,7 @@
       </c>
       <c r="G34">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -7044,7 +7105,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -7073,7 +7134,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="5"/>
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -7102,7 +7163,7 @@
       </c>
       <c r="G37">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -7131,7 +7192,7 @@
       </c>
       <c r="G38">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -7160,7 +7221,7 @@
       </c>
       <c r="G39">
         <f t="shared" si="5"/>
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -7189,7 +7250,7 @@
       </c>
       <c r="G40">
         <f t="shared" si="5"/>
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -7218,7 +7279,7 @@
       </c>
       <c r="G41">
         <f t="shared" si="5"/>
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -7247,7 +7308,7 @@
       </c>
       <c r="G42">
         <f t="shared" si="5"/>
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -7276,7 +7337,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="5"/>
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -7305,7 +7366,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="5"/>
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -7334,7 +7395,7 @@
       </c>
       <c r="G45">
         <f t="shared" si="5"/>
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -7363,7 +7424,7 @@
       </c>
       <c r="G46">
         <f t="shared" si="5"/>
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -7392,7 +7453,7 @@
       </c>
       <c r="G47">
         <f t="shared" si="5"/>
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -7421,7 +7482,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="5"/>
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -7450,7 +7511,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="5"/>
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -7479,7 +7540,7 @@
       </c>
       <c r="G50">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -7508,7 +7569,7 @@
       </c>
       <c r="G51">
         <f t="shared" si="5"/>
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -7537,7 +7598,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="5"/>
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -7566,7 +7627,7 @@
       </c>
       <c r="G53">
         <f t="shared" si="5"/>
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -7595,7 +7656,7 @@
       </c>
       <c r="G54">
         <f t="shared" si="5"/>
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -7624,7 +7685,7 @@
       </c>
       <c r="G55">
         <f t="shared" si="5"/>
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -7653,7 +7714,7 @@
       </c>
       <c r="G56">
         <f t="shared" si="5"/>
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -7682,7 +7743,7 @@
       </c>
       <c r="G57">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -7711,7 +7772,7 @@
       </c>
       <c r="G58">
         <f t="shared" si="5"/>
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -7740,7 +7801,7 @@
       </c>
       <c r="G59">
         <f t="shared" si="5"/>
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -7769,7 +7830,7 @@
       </c>
       <c r="G60">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -7798,7 +7859,7 @@
       </c>
       <c r="G61">
         <f t="shared" si="5"/>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -7827,7 +7888,7 @@
       </c>
       <c r="G62">
         <f t="shared" si="5"/>
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -7856,7 +7917,7 @@
       </c>
       <c r="G63">
         <f t="shared" si="5"/>
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -7885,7 +7946,7 @@
       </c>
       <c r="G64">
         <f t="shared" si="5"/>
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -7914,7 +7975,7 @@
       </c>
       <c r="G65">
         <f t="shared" si="5"/>
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -7943,7 +8004,7 @@
       </c>
       <c r="G66">
         <f t="shared" si="5"/>
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -7972,7 +8033,7 @@
       </c>
       <c r="G67">
         <f t="shared" si="5"/>
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -8001,7 +8062,7 @@
       </c>
       <c r="G68">
         <f t="shared" si="5"/>
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -8030,7 +8091,7 @@
       </c>
       <c r="G69">
         <f t="shared" ref="G69:G132" si="11">ROUND(D69*$G$2,0)</f>
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -8059,7 +8120,7 @@
       </c>
       <c r="G70">
         <f t="shared" si="11"/>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -8088,7 +8149,7 @@
       </c>
       <c r="G71">
         <f t="shared" si="11"/>
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -8117,7 +8178,7 @@
       </c>
       <c r="G72">
         <f t="shared" si="11"/>
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -8146,7 +8207,7 @@
       </c>
       <c r="G73">
         <f t="shared" si="11"/>
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -8175,7 +8236,7 @@
       </c>
       <c r="G74">
         <f t="shared" si="11"/>
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -8204,7 +8265,7 @@
       </c>
       <c r="G75">
         <f t="shared" si="11"/>
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -8233,7 +8294,7 @@
       </c>
       <c r="G76">
         <f t="shared" si="11"/>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -8262,7 +8323,7 @@
       </c>
       <c r="G77">
         <f t="shared" si="11"/>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -8320,7 +8381,7 @@
       </c>
       <c r="G79">
         <f t="shared" si="11"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -8349,7 +8410,7 @@
       </c>
       <c r="G80">
         <f t="shared" si="11"/>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -8407,7 +8468,7 @@
       </c>
       <c r="G82">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -8436,7 +8497,7 @@
       </c>
       <c r="G83">
         <f t="shared" si="11"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -8610,7 +8671,7 @@
       </c>
       <c r="G89">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -8639,7 +8700,7 @@
       </c>
       <c r="G90">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -8813,7 +8874,7 @@
       </c>
       <c r="G96">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -10843,7 +10904,7 @@
       </c>
       <c r="G166">
         <f t="shared" si="17"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -11017,7 +11078,7 @@
       </c>
       <c r="G172">
         <f t="shared" si="17"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -11046,7 +11107,7 @@
       </c>
       <c r="G173">
         <f t="shared" si="17"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -11220,7 +11281,7 @@
       </c>
       <c r="G179">
         <f t="shared" si="17"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -11249,7 +11310,7 @@
       </c>
       <c r="G180">
         <f t="shared" si="17"/>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -11307,7 +11368,7 @@
       </c>
       <c r="G182">
         <f t="shared" si="17"/>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -11336,7 +11397,7 @@
       </c>
       <c r="G183">
         <f t="shared" si="17"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -11394,7 +11455,7 @@
       </c>
       <c r="G185">
         <f t="shared" si="17"/>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -11423,7 +11484,7 @@
       </c>
       <c r="G186">
         <f t="shared" si="17"/>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -11452,7 +11513,7 @@
       </c>
       <c r="G187">
         <f t="shared" si="17"/>
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -11481,7 +11542,7 @@
       </c>
       <c r="G188">
         <f t="shared" si="17"/>
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -11510,7 +11571,7 @@
       </c>
       <c r="G189">
         <f t="shared" si="17"/>
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -11539,7 +11600,7 @@
       </c>
       <c r="G190">
         <f t="shared" si="17"/>
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -11568,7 +11629,7 @@
       </c>
       <c r="G191">
         <f t="shared" si="17"/>
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -11597,7 +11658,7 @@
       </c>
       <c r="G192">
         <f t="shared" si="17"/>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -11626,7 +11687,7 @@
       </c>
       <c r="G193">
         <f t="shared" si="17"/>
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -11655,7 +11716,7 @@
       </c>
       <c r="G194">
         <f t="shared" si="17"/>
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -11684,7 +11745,7 @@
       </c>
       <c r="G195">
         <f t="shared" si="17"/>
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -11713,7 +11774,7 @@
       </c>
       <c r="G196">
         <f t="shared" si="17"/>
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -11742,7 +11803,7 @@
       </c>
       <c r="G197">
         <f t="shared" ref="G197:G259" si="23">ROUND(D197*$G$2,0)</f>
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -11771,7 +11832,7 @@
       </c>
       <c r="G198">
         <f t="shared" si="23"/>
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -11800,7 +11861,7 @@
       </c>
       <c r="G199">
         <f t="shared" si="23"/>
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -11829,7 +11890,7 @@
       </c>
       <c r="G200">
         <f t="shared" si="23"/>
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -11858,7 +11919,7 @@
       </c>
       <c r="G201">
         <f t="shared" si="23"/>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -11887,7 +11948,7 @@
       </c>
       <c r="G202">
         <f t="shared" si="23"/>
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -11916,7 +11977,7 @@
       </c>
       <c r="G203">
         <f t="shared" si="23"/>
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -11945,7 +12006,7 @@
       </c>
       <c r="G204">
         <f t="shared" si="23"/>
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -11974,7 +12035,7 @@
       </c>
       <c r="G205">
         <f t="shared" si="23"/>
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -12003,7 +12064,7 @@
       </c>
       <c r="G206">
         <f t="shared" si="23"/>
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -12032,7 +12093,7 @@
       </c>
       <c r="G207">
         <f t="shared" si="23"/>
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -12061,7 +12122,7 @@
       </c>
       <c r="G208">
         <f t="shared" si="23"/>
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -12090,7 +12151,7 @@
       </c>
       <c r="G209">
         <f t="shared" si="23"/>
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -12119,7 +12180,7 @@
       </c>
       <c r="G210">
         <f t="shared" si="23"/>
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -12148,7 +12209,7 @@
       </c>
       <c r="G211">
         <f t="shared" si="23"/>
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -12177,7 +12238,7 @@
       </c>
       <c r="G212">
         <f t="shared" si="23"/>
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -12206,7 +12267,7 @@
       </c>
       <c r="G213">
         <f t="shared" si="23"/>
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -12235,7 +12296,7 @@
       </c>
       <c r="G214">
         <f t="shared" si="23"/>
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -12264,7 +12325,7 @@
       </c>
       <c r="G215">
         <f t="shared" si="23"/>
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -12293,7 +12354,7 @@
       </c>
       <c r="G216">
         <f t="shared" si="23"/>
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -12322,7 +12383,7 @@
       </c>
       <c r="G217">
         <f t="shared" si="23"/>
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -12351,7 +12412,7 @@
       </c>
       <c r="G218">
         <f t="shared" si="23"/>
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -12380,7 +12441,7 @@
       </c>
       <c r="G219">
         <f t="shared" si="23"/>
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -12409,7 +12470,7 @@
       </c>
       <c r="G220">
         <f t="shared" si="23"/>
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -12438,7 +12499,7 @@
       </c>
       <c r="G221">
         <f t="shared" si="23"/>
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -12467,7 +12528,7 @@
       </c>
       <c r="G222">
         <f t="shared" si="23"/>
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -12496,7 +12557,7 @@
       </c>
       <c r="G223">
         <f t="shared" si="23"/>
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -12525,7 +12586,7 @@
       </c>
       <c r="G224">
         <f t="shared" si="23"/>
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -12554,7 +12615,7 @@
       </c>
       <c r="G225">
         <f t="shared" si="23"/>
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -12583,7 +12644,7 @@
       </c>
       <c r="G226">
         <f t="shared" si="23"/>
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -12612,7 +12673,7 @@
       </c>
       <c r="G227">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -12641,7 +12702,7 @@
       </c>
       <c r="G228">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -12670,7 +12731,7 @@
       </c>
       <c r="G229">
         <f t="shared" si="23"/>
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -12699,7 +12760,7 @@
       </c>
       <c r="G230">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -12728,7 +12789,7 @@
       </c>
       <c r="G231">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -12757,7 +12818,7 @@
       </c>
       <c r="G232">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -12786,7 +12847,7 @@
       </c>
       <c r="G233">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -12815,7 +12876,7 @@
       </c>
       <c r="G234">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -12844,7 +12905,7 @@
       </c>
       <c r="G235">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -12873,7 +12934,7 @@
       </c>
       <c r="G236">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -12902,7 +12963,7 @@
       </c>
       <c r="G237">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -12931,7 +12992,7 @@
       </c>
       <c r="G238">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -12960,7 +13021,7 @@
       </c>
       <c r="G239">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -12989,7 +13050,7 @@
       </c>
       <c r="G240">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -13018,7 +13079,7 @@
       </c>
       <c r="G241">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -13047,7 +13108,7 @@
       </c>
       <c r="G242">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -13076,7 +13137,7 @@
       </c>
       <c r="G243">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -13105,7 +13166,7 @@
       </c>
       <c r="G244">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -13134,7 +13195,7 @@
       </c>
       <c r="G245">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -13163,7 +13224,7 @@
       </c>
       <c r="G246">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -13192,7 +13253,7 @@
       </c>
       <c r="G247">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -13221,7 +13282,7 @@
       </c>
       <c r="G248">
         <f t="shared" si="23"/>
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -13250,7 +13311,7 @@
       </c>
       <c r="G249">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -13279,7 +13340,7 @@
       </c>
       <c r="G250">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -13308,7 +13369,7 @@
       </c>
       <c r="G251">
         <f t="shared" si="23"/>
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -13337,7 +13398,7 @@
       </c>
       <c r="G252">
         <f t="shared" si="23"/>
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -13366,7 +13427,7 @@
       </c>
       <c r="G253">
         <f t="shared" si="23"/>
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -13395,7 +13456,7 @@
       </c>
       <c r="G254">
         <f t="shared" si="23"/>
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -13424,7 +13485,7 @@
       </c>
       <c r="G255">
         <f t="shared" si="23"/>
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -13453,7 +13514,7 @@
       </c>
       <c r="G256">
         <f t="shared" si="23"/>
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -13482,7 +13543,7 @@
       </c>
       <c r="G257">
         <f t="shared" si="23"/>
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -13511,7 +13572,7 @@
       </c>
       <c r="G258">
         <f t="shared" si="23"/>
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -13540,7 +13601,7 @@
       </c>
       <c r="G259">
         <f t="shared" si="23"/>
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 14 - motor_controller() loop removed - FOC Angle calculation algorithm changed - Field Weakening Enable/Disable
</commit_message>
<xml_diff>
--- a/CSV-PWM-Table.xlsx
+++ b/CSV-PWM-Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-Smart-EBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF822B2C-A627-4287-B98B-27BF02E2BA50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE218C7-A457-40F7-AE34-298ECB9DE0F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="324" windowWidth="18972" windowHeight="11136" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
+    <workbookView xWindow="384" yWindow="324" windowWidth="21204" windowHeight="11568" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
   </bookViews>
   <sheets>
     <sheet name="Midpoint Clamp (CSV PWM)" sheetId="2" r:id="rId1"/>
@@ -6096,7 +6096,7 @@
   <dimension ref="A1:M259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6138,8 +6138,8 @@
         <v>0.86629626434835505</v>
       </c>
       <c r="G2">
-        <f>H2/2-7</f>
-        <v>215</v>
+        <f>H2/2-1</f>
+        <v>221</v>
       </c>
       <c r="H2" s="6">
         <v>444</v>
@@ -6150,11 +6150,11 @@
       </c>
       <c r="L2">
         <f>TRUNC(254*G2/256)</f>
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="M2">
         <f>H2/2-L2</f>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -6194,7 +6194,7 @@
       </c>
       <c r="G4">
         <f>ROUND(D4*$G$2,0)</f>
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -6223,7 +6223,7 @@
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G68" si="5">ROUND(D5*$G$2,0)</f>
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="5"/>
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -6281,7 +6281,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -6310,7 +6310,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="5"/>
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -6339,7 +6339,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="5"/>
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -6397,7 +6397,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -6455,7 +6455,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -6484,7 +6484,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -6513,7 +6513,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -6600,7 +6600,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -6629,7 +6629,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -6658,7 +6658,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -6687,7 +6687,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -6716,7 +6716,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -6745,7 +6745,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -6774,7 +6774,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -6832,7 +6832,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -6890,7 +6890,7 @@
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I28" t="s">
         <v>6</v>
@@ -6922,7 +6922,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I29" t="s">
         <v>5</v>
@@ -6954,7 +6954,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="5"/>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I30" t="s">
         <v>4</v>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="I31" t="s">
         <v>1</v>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -7076,7 +7076,7 @@
       </c>
       <c r="G34">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -7105,7 +7105,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="5"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -7134,7 +7134,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -7163,7 +7163,7 @@
       </c>
       <c r="G37">
         <f t="shared" si="5"/>
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -7192,7 +7192,7 @@
       </c>
       <c r="G38">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -7221,7 +7221,7 @@
       </c>
       <c r="G39">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -7250,7 +7250,7 @@
       </c>
       <c r="G40">
         <f t="shared" si="5"/>
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -7279,7 +7279,7 @@
       </c>
       <c r="G41">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -7308,7 +7308,7 @@
       </c>
       <c r="G42">
         <f t="shared" si="5"/>
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -7337,7 +7337,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="5"/>
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="5"/>
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -7395,7 +7395,7 @@
       </c>
       <c r="G45">
         <f t="shared" si="5"/>
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -7424,7 +7424,7 @@
       </c>
       <c r="G46">
         <f t="shared" si="5"/>
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -7453,7 +7453,7 @@
       </c>
       <c r="G47">
         <f t="shared" si="5"/>
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -7482,7 +7482,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="5"/>
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -7511,7 +7511,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="5"/>
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -7540,7 +7540,7 @@
       </c>
       <c r="G50">
         <f t="shared" si="5"/>
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -7569,7 +7569,7 @@
       </c>
       <c r="G51">
         <f t="shared" si="5"/>
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="5"/>
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -7627,7 +7627,7 @@
       </c>
       <c r="G53">
         <f t="shared" si="5"/>
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -7656,7 +7656,7 @@
       </c>
       <c r="G54">
         <f t="shared" si="5"/>
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -7685,7 +7685,7 @@
       </c>
       <c r="G55">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -7714,7 +7714,7 @@
       </c>
       <c r="G56">
         <f t="shared" si="5"/>
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -7743,7 +7743,7 @@
       </c>
       <c r="G57">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -7772,7 +7772,7 @@
       </c>
       <c r="G58">
         <f t="shared" si="5"/>
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -7801,7 +7801,7 @@
       </c>
       <c r="G59">
         <f t="shared" si="5"/>
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -7830,7 +7830,7 @@
       </c>
       <c r="G60">
         <f t="shared" si="5"/>
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -7859,7 +7859,7 @@
       </c>
       <c r="G61">
         <f t="shared" si="5"/>
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -7888,7 +7888,7 @@
       </c>
       <c r="G62">
         <f t="shared" si="5"/>
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -7917,7 +7917,7 @@
       </c>
       <c r="G63">
         <f t="shared" si="5"/>
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -7946,7 +7946,7 @@
       </c>
       <c r="G64">
         <f t="shared" si="5"/>
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -7975,7 +7975,7 @@
       </c>
       <c r="G65">
         <f t="shared" si="5"/>
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -8004,7 +8004,7 @@
       </c>
       <c r="G66">
         <f t="shared" si="5"/>
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="G67">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -8062,7 +8062,7 @@
       </c>
       <c r="G68">
         <f t="shared" si="5"/>
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -8091,7 +8091,7 @@
       </c>
       <c r="G69">
         <f t="shared" ref="G69:G132" si="11">ROUND(D69*$G$2,0)</f>
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -8120,7 +8120,7 @@
       </c>
       <c r="G70">
         <f t="shared" si="11"/>
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="G71">
         <f t="shared" si="11"/>
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -8178,7 +8178,7 @@
       </c>
       <c r="G72">
         <f t="shared" si="11"/>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -8207,7 +8207,7 @@
       </c>
       <c r="G73">
         <f t="shared" si="11"/>
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="G74">
         <f t="shared" si="11"/>
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -8265,7 +8265,7 @@
       </c>
       <c r="G75">
         <f t="shared" si="11"/>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="G76">
         <f t="shared" si="11"/>
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -8323,7 +8323,7 @@
       </c>
       <c r="G77">
         <f t="shared" si="11"/>
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -8352,7 +8352,7 @@
       </c>
       <c r="G78">
         <f t="shared" si="11"/>
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -8381,7 +8381,7 @@
       </c>
       <c r="G79">
         <f t="shared" si="11"/>
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -8410,7 +8410,7 @@
       </c>
       <c r="G80">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="G81">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -8468,7 +8468,7 @@
       </c>
       <c r="G82">
         <f t="shared" si="11"/>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -8497,7 +8497,7 @@
       </c>
       <c r="G83">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -8526,7 +8526,7 @@
       </c>
       <c r="G84">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="G85">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -8584,7 +8584,7 @@
       </c>
       <c r="G86">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -8729,7 +8729,7 @@
       </c>
       <c r="G91">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -8758,7 +8758,7 @@
       </c>
       <c r="G92">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -8787,7 +8787,7 @@
       </c>
       <c r="G93">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -8816,7 +8816,7 @@
       </c>
       <c r="G94">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="G95">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -9802,7 +9802,7 @@
       </c>
       <c r="G128">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -9889,7 +9889,7 @@
       </c>
       <c r="G131">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -9976,7 +9976,7 @@
       </c>
       <c r="G134">
         <f t="shared" si="17"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -10933,7 +10933,7 @@
       </c>
       <c r="G167">
         <f t="shared" si="17"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -10962,7 +10962,7 @@
       </c>
       <c r="G168">
         <f t="shared" si="17"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="G169">
         <f t="shared" si="17"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -11020,7 +11020,7 @@
       </c>
       <c r="G170">
         <f t="shared" si="17"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -11049,7 +11049,7 @@
       </c>
       <c r="G171">
         <f t="shared" si="17"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -11194,7 +11194,7 @@
       </c>
       <c r="G176">
         <f t="shared" si="17"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -11223,7 +11223,7 @@
       </c>
       <c r="G177">
         <f t="shared" si="17"/>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -11252,7 +11252,7 @@
       </c>
       <c r="G178">
         <f t="shared" si="17"/>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -11281,7 +11281,7 @@
       </c>
       <c r="G179">
         <f t="shared" si="17"/>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -11310,7 +11310,7 @@
       </c>
       <c r="G180">
         <f t="shared" si="17"/>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -11339,7 +11339,7 @@
       </c>
       <c r="G181">
         <f t="shared" si="17"/>
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -11368,7 +11368,7 @@
       </c>
       <c r="G182">
         <f t="shared" si="17"/>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -11397,7 +11397,7 @@
       </c>
       <c r="G183">
         <f t="shared" si="17"/>
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -11426,7 +11426,7 @@
       </c>
       <c r="G184">
         <f t="shared" si="17"/>
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -11455,7 +11455,7 @@
       </c>
       <c r="G185">
         <f t="shared" si="17"/>
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -11484,7 +11484,7 @@
       </c>
       <c r="G186">
         <f t="shared" si="17"/>
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="G187">
         <f t="shared" si="17"/>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -11542,7 +11542,7 @@
       </c>
       <c r="G188">
         <f t="shared" si="17"/>
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -11571,7 +11571,7 @@
       </c>
       <c r="G189">
         <f t="shared" si="17"/>
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -11600,7 +11600,7 @@
       </c>
       <c r="G190">
         <f t="shared" si="17"/>
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -11629,7 +11629,7 @@
       </c>
       <c r="G191">
         <f t="shared" si="17"/>
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -11658,7 +11658,7 @@
       </c>
       <c r="G192">
         <f t="shared" si="17"/>
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -11687,7 +11687,7 @@
       </c>
       <c r="G193">
         <f t="shared" si="17"/>
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -11716,7 +11716,7 @@
       </c>
       <c r="G194">
         <f t="shared" si="17"/>
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -11745,7 +11745,7 @@
       </c>
       <c r="G195">
         <f t="shared" si="17"/>
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -11774,7 +11774,7 @@
       </c>
       <c r="G196">
         <f t="shared" si="17"/>
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -11803,7 +11803,7 @@
       </c>
       <c r="G197">
         <f t="shared" ref="G197:G259" si="23">ROUND(D197*$G$2,0)</f>
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -11832,7 +11832,7 @@
       </c>
       <c r="G198">
         <f t="shared" si="23"/>
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -11861,7 +11861,7 @@
       </c>
       <c r="G199">
         <f t="shared" si="23"/>
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -11890,7 +11890,7 @@
       </c>
       <c r="G200">
         <f t="shared" si="23"/>
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -11919,7 +11919,7 @@
       </c>
       <c r="G201">
         <f t="shared" si="23"/>
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -11948,7 +11948,7 @@
       </c>
       <c r="G202">
         <f t="shared" si="23"/>
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -11977,7 +11977,7 @@
       </c>
       <c r="G203">
         <f t="shared" si="23"/>
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -12006,7 +12006,7 @@
       </c>
       <c r="G204">
         <f t="shared" si="23"/>
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -12035,7 +12035,7 @@
       </c>
       <c r="G205">
         <f t="shared" si="23"/>
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -12064,7 +12064,7 @@
       </c>
       <c r="G206">
         <f t="shared" si="23"/>
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -12093,7 +12093,7 @@
       </c>
       <c r="G207">
         <f t="shared" si="23"/>
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -12122,7 +12122,7 @@
       </c>
       <c r="G208">
         <f t="shared" si="23"/>
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -12151,7 +12151,7 @@
       </c>
       <c r="G209">
         <f t="shared" si="23"/>
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -12180,7 +12180,7 @@
       </c>
       <c r="G210">
         <f t="shared" si="23"/>
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -12209,7 +12209,7 @@
       </c>
       <c r="G211">
         <f t="shared" si="23"/>
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -12238,7 +12238,7 @@
       </c>
       <c r="G212">
         <f t="shared" si="23"/>
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -12267,7 +12267,7 @@
       </c>
       <c r="G213">
         <f t="shared" si="23"/>
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -12296,7 +12296,7 @@
       </c>
       <c r="G214">
         <f t="shared" si="23"/>
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -12325,7 +12325,7 @@
       </c>
       <c r="G215">
         <f t="shared" si="23"/>
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -12354,7 +12354,7 @@
       </c>
       <c r="G216">
         <f t="shared" si="23"/>
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="G217">
         <f t="shared" si="23"/>
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -12412,7 +12412,7 @@
       </c>
       <c r="G218">
         <f t="shared" si="23"/>
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -12441,7 +12441,7 @@
       </c>
       <c r="G219">
         <f t="shared" si="23"/>
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -12470,7 +12470,7 @@
       </c>
       <c r="G220">
         <f t="shared" si="23"/>
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -12499,7 +12499,7 @@
       </c>
       <c r="G221">
         <f t="shared" si="23"/>
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -12528,7 +12528,7 @@
       </c>
       <c r="G222">
         <f t="shared" si="23"/>
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -12557,7 +12557,7 @@
       </c>
       <c r="G223">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -12586,7 +12586,7 @@
       </c>
       <c r="G224">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -12615,7 +12615,7 @@
       </c>
       <c r="G225">
         <f t="shared" si="23"/>
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -12644,7 +12644,7 @@
       </c>
       <c r="G226">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="G227">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -12702,7 +12702,7 @@
       </c>
       <c r="G228">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -12731,7 +12731,7 @@
       </c>
       <c r="G229">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -12760,7 +12760,7 @@
       </c>
       <c r="G230">
         <f t="shared" si="23"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -12789,7 +12789,7 @@
       </c>
       <c r="G231">
         <f t="shared" si="23"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -12818,7 +12818,7 @@
       </c>
       <c r="G232">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -12847,7 +12847,7 @@
       </c>
       <c r="G233">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -12876,7 +12876,7 @@
       </c>
       <c r="G234">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -12905,7 +12905,7 @@
       </c>
       <c r="G235">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -12934,7 +12934,7 @@
       </c>
       <c r="G236">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -12963,7 +12963,7 @@
       </c>
       <c r="G237">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -12992,7 +12992,7 @@
       </c>
       <c r="G238">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -13021,7 +13021,7 @@
       </c>
       <c r="G239">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="G240">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -13079,7 +13079,7 @@
       </c>
       <c r="G241">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -13108,7 +13108,7 @@
       </c>
       <c r="G242">
         <f t="shared" si="23"/>
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -13137,7 +13137,7 @@
       </c>
       <c r="G243">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -13166,7 +13166,7 @@
       </c>
       <c r="G244">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -13195,7 +13195,7 @@
       </c>
       <c r="G245">
         <f t="shared" si="23"/>
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -13224,7 +13224,7 @@
       </c>
       <c r="G246">
         <f t="shared" si="23"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -13253,7 +13253,7 @@
       </c>
       <c r="G247">
         <f t="shared" si="23"/>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -13282,7 +13282,7 @@
       </c>
       <c r="G248">
         <f t="shared" si="23"/>
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -13311,7 +13311,7 @@
       </c>
       <c r="G249">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -13340,7 +13340,7 @@
       </c>
       <c r="G250">
         <f t="shared" si="23"/>
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -13369,7 +13369,7 @@
       </c>
       <c r="G251">
         <f t="shared" si="23"/>
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -13398,7 +13398,7 @@
       </c>
       <c r="G252">
         <f t="shared" si="23"/>
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -13427,7 +13427,7 @@
       </c>
       <c r="G253">
         <f t="shared" si="23"/>
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -13456,7 +13456,7 @@
       </c>
       <c r="G254">
         <f t="shared" si="23"/>
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -13485,7 +13485,7 @@
       </c>
       <c r="G255">
         <f t="shared" si="23"/>
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -13514,7 +13514,7 @@
       </c>
       <c r="G256">
         <f t="shared" si="23"/>
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -13543,7 +13543,7 @@
       </c>
       <c r="G257">
         <f t="shared" si="23"/>
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -13572,7 +13572,7 @@
       </c>
       <c r="G258">
         <f t="shared" si="23"/>
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -13601,7 +13601,7 @@
       </c>
       <c r="G259">
         <f t="shared" si="23"/>
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>